<commit_message>
Add and update various agenda and journal files; remove outdated entries
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/01-january-hh/resident-directory/2025-01-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/01-january-hh/resident-directory/2025-01-heritage-resident-directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/01-january-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="759" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F01F875A-7C72-497E-B060-5C12C0DAA925}"/>
+  <xr:revisionPtr revIDLastSave="760" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A51410A4-3B71-4189-AB6E-8364991738FE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="1093">
   <si>
     <t>First Name</t>
   </si>
@@ -3322,15 +3322,6 @@
   </si>
   <si>
     <t>donna@nextvillagesf.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diana </t>
-  </si>
-  <si>
-    <t>Greer</t>
-  </si>
-  <si>
-    <t>diana94133@pm.me</t>
   </si>
   <si>
     <t>martynolan40@gmail.com</t>
@@ -3963,10 +3954,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4191,7 +4178,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -5588,7 +5575,7 @@
         <v>293</v>
       </c>
       <c r="F56" s="52" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -8923,7 +8910,7 @@
   </sheetPr>
   <dimension ref="A2:K36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -8938,7 +8925,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -12966,7 +12953,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>1030</v>
@@ -13686,7 +13673,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>1038</v>
@@ -13805,7 +13792,7 @@
         <v>302</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>301</v>
@@ -14207,7 +14194,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -14521,11 +14508,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA4147-474C-47CD-A0DD-4C67000E8368}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71:D74"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -14541,7 +14528,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>632</v>
@@ -15300,7 +15287,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>751</v>
@@ -15311,57 +15298,46 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>1084</v>
+        <v>1074</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>1086</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
-        <v>1074</v>
+        <v>1080</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>1079</v>
+        <v>1011</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1011</v>
+        <v>1082</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="11" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>1094</v>
+        <v>1090</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>1091</v>
       </c>
     </row>
   </sheetData>
@@ -15396,7 +15372,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>632</v>
@@ -15866,7 +15842,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>632</v>
@@ -16066,7 +16042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C4CAD2-851C-4D78-8B2D-D5100B32C514}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
@@ -16084,7 +16060,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -16104,7 +16080,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>34</v>

</xml_diff>